<commit_message>
Updated data for demographics.
</commit_message>
<xml_diff>
--- a/output/01-overall.xlsx
+++ b/output/01-overall.xlsx
@@ -354,7 +354,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -405,57 +405,225 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>NS</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="B2">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C2">
-        <v>845</v>
+        <v>481</v>
       </c>
       <c r="D2">
-        <v>0.008185638647955082</v>
+        <v>0.009547402667062702</v>
       </c>
       <c r="E2">
-        <v>0.05062140192408826</v>
+        <v>0.05049913521583405</v>
       </c>
       <c r="F2">
-        <v>97.74010293942425</v>
+        <v>97.23510890274069</v>
       </c>
       <c r="G2">
-        <v>84.13518155087188</v>
+        <v>81.77472149654884</v>
       </c>
       <c r="H2">
-        <v>13.60492138855237</v>
+        <v>15.46038740619185</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>AT</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>47</v>
+      </c>
+      <c r="C3">
+        <v>278</v>
+      </c>
+      <c r="D3">
+        <v>0.007326863613329796</v>
+      </c>
+      <c r="E3">
+        <v>0.05416945844946475</v>
+      </c>
+      <c r="F3">
+        <v>95.22131472033337</v>
+      </c>
+      <c r="G3">
+        <v>83.87635029586855</v>
+      </c>
+      <c r="H3">
+        <v>11.34496442446483</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CS</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>21</v>
+      </c>
+      <c r="C4">
+        <v>124</v>
+      </c>
+      <c r="D4">
+        <v>1.731237972880323e-10</v>
+      </c>
+      <c r="E4">
+        <v>0.05347177606605178</v>
+      </c>
+      <c r="F4">
+        <v>94.56480169864874</v>
+      </c>
+      <c r="G4">
+        <v>94.56480139247941</v>
+      </c>
+      <c r="H4">
+        <v>3.061693235442865e-07</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>CT</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>64</v>
+      </c>
+      <c r="D5">
+        <v>1.180464018637195e-11</v>
+      </c>
+      <c r="E5">
+        <v>0.05686279483535307</v>
+      </c>
+      <c r="F5">
+        <v>93.66722064194497</v>
+      </c>
+      <c r="G5">
+        <v>93.66722062249977</v>
+      </c>
+      <c r="H5">
+        <v>1.94451897749261e-08</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>NS</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>67</v>
+      </c>
+      <c r="D6">
+        <v>0.002568221237042442</v>
+      </c>
+      <c r="E6">
+        <v>0.08196038047578791</v>
+      </c>
+      <c r="F6">
+        <v>97.72915636699312</v>
+      </c>
+      <c r="G6">
+        <v>94.75986443770458</v>
+      </c>
+      <c r="H6">
+        <v>2.969291929288548</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>NT</t>
         </is>
       </c>
-      <c r="B3">
-        <v>51</v>
-      </c>
-      <c r="C3">
-        <v>438</v>
-      </c>
-      <c r="D3">
-        <v>0.003055542066856273</v>
-      </c>
-      <c r="E3">
-        <v>0.05309002432744785</v>
-      </c>
-      <c r="F3">
-        <v>95.03669962100878</v>
-      </c>
-      <c r="G3">
-        <v>89.86463257749891</v>
-      </c>
-      <c r="H3">
-        <v>5.172067043509874</v>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>2.160635946778273e-09</v>
+      </c>
+      <c r="E7">
+        <v>0.104042481579473</v>
+      </c>
+      <c r="F7">
+        <v>98.19513126041213</v>
+      </c>
+      <c r="G7">
+        <v>98.19512922120734</v>
+      </c>
+      <c r="H7">
+        <v>2.039204782248648e-06</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>RS</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>69</v>
+      </c>
+      <c r="D8">
+        <v>0.003443972131837947</v>
+      </c>
+      <c r="E8">
+        <v>0.06418092805950022</v>
+      </c>
+      <c r="F8">
+        <v>95.41107325558967</v>
+      </c>
+      <c r="G8">
+        <v>90.55201872935338</v>
+      </c>
+      <c r="H8">
+        <v>4.859054526236299</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>RT</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>26</v>
+      </c>
+      <c r="D9">
+        <v>0.003974260035750185</v>
+      </c>
+      <c r="E9">
+        <v>0.04112607210659971</v>
+      </c>
+      <c r="F9">
+        <v>93.57203529029329</v>
+      </c>
+      <c r="G9">
+        <v>85.32642860286896</v>
+      </c>
+      <c r="H9">
+        <v>8.245606687424328</v>
       </c>
     </row>
   </sheetData>
@@ -465,7 +633,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -526,7 +694,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>NS</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -540,63 +708,291 @@
         </is>
       </c>
       <c r="D2">
-        <v>0.1084666938471611</v>
+        <v>0.115859125074652</v>
       </c>
       <c r="E2">
-        <v>0.01613508533834829</v>
+        <v>0.019311310921687</v>
       </c>
       <c r="F2">
-        <v>6.748962946546104</v>
+        <v>6.026610342222342</v>
       </c>
       <c r="G2">
-        <v>3.624994104290959e-09</v>
+        <v>1.116457001585076e-07</v>
       </c>
       <c r="H2">
-        <v>0.07656241013489337</v>
+        <v>0.07759536281618994</v>
       </c>
       <c r="I2">
-        <v>0.140149089876684</v>
+        <v>0.1537820719809943</v>
       </c>
       <c r="J2">
-        <v>69.73578864538069</v>
+        <v>59.87113439968061</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>AT</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>summary</t>
+        </is>
+      </c>
+      <c r="D3">
+        <v>0.06170936389133818</v>
+      </c>
+      <c r="E3">
+        <v>0.02267082070753755</v>
+      </c>
+      <c r="F3">
+        <v>2.725436138336921</v>
+      </c>
+      <c r="G3">
+        <v>0.009455249671854219</v>
+      </c>
+      <c r="H3">
+        <v>0.01597812901652559</v>
+      </c>
+      <c r="I3">
+        <v>0.1071829605582368</v>
+      </c>
+      <c r="J3">
+        <v>40.31224445286919</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CS</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>summary</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>0.1069656926610476</v>
+      </c>
+      <c r="E4">
+        <v>0.02418197627559185</v>
+      </c>
+      <c r="F4">
+        <v>4.440351365349607</v>
+      </c>
+      <c r="G4">
+        <v>0.0004652046791313454</v>
+      </c>
+      <c r="H4">
+        <v>0.05582347336609818</v>
+      </c>
+      <c r="I4">
+        <v>0.1575480884058547</v>
+      </c>
+      <c r="J4">
+        <v>15.1614384244598</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>CT</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>summary</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>0.02781729689565586</v>
+      </c>
+      <c r="E5">
+        <v>0.01842241430203381</v>
+      </c>
+      <c r="F5">
+        <v>1.510359869193418</v>
+      </c>
+      <c r="G5">
+        <v>0.1653270565126447</v>
+      </c>
+      <c r="H5">
+        <v>-0.01386669229402327</v>
+      </c>
+      <c r="I5">
+        <v>0.06940476706915732</v>
+      </c>
+      <c r="J5">
+        <v>8.97505936890877</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>NS</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>summary</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>0.1543627352939112</v>
+      </c>
+      <c r="E6">
+        <v>0.0435122887447019</v>
+      </c>
+      <c r="F6">
+        <v>3.57615322930177</v>
+      </c>
+      <c r="G6">
+        <v>0.006038254960428799</v>
+      </c>
+      <c r="H6">
+        <v>0.05700144922515708</v>
+      </c>
+      <c r="I6">
+        <v>0.2488156639258952</v>
+      </c>
+      <c r="J6">
+        <v>8.933579212714715</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>NT</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>overall</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>summary</t>
         </is>
       </c>
-      <c r="D3">
-        <v>0.04705522139931226</v>
-      </c>
-      <c r="E3">
-        <v>0.01749867517286095</v>
-      </c>
-      <c r="F3">
-        <v>2.691060719765634</v>
-      </c>
-      <c r="G3">
-        <v>0.01016425005378666</v>
-      </c>
-      <c r="H3">
-        <v>0.0117807924887667</v>
-      </c>
-      <c r="I3">
-        <v>0.08221267937717935</v>
-      </c>
-      <c r="J3">
-        <v>42.20562044925089</v>
+      <c r="D7">
+        <v>0.09175852176935832</v>
+      </c>
+      <c r="E7">
+        <v>0.05176709047110706</v>
+      </c>
+      <c r="F7">
+        <v>1.777526106194264</v>
+      </c>
+      <c r="G7">
+        <v>0.2003309063696341</v>
+      </c>
+      <c r="H7">
+        <v>-0.1041016045915139</v>
+      </c>
+      <c r="I7">
+        <v>0.2807672931239559</v>
+      </c>
+      <c r="J7">
+        <v>2.308657586752851</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>RS</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>summary</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>0.1307611718375587</v>
+      </c>
+      <c r="E8">
+        <v>0.04351490228835033</v>
+      </c>
+      <c r="F8">
+        <v>3.022279218936637</v>
+      </c>
+      <c r="G8">
+        <v>0.0202660674140272</v>
+      </c>
+      <c r="H8">
+        <v>0.02776580867556062</v>
+      </c>
+      <c r="I8">
+        <v>0.2310093189054091</v>
+      </c>
+      <c r="J8">
+        <v>6.729369212196717</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>RT</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>summary</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>0.01292644007739949</v>
+      </c>
+      <c r="E9">
+        <v>0.0596240423909054</v>
+      </c>
+      <c r="F9">
+        <v>0.2168111990252905</v>
+      </c>
+      <c r="G9">
+        <v>0.8413778317361429</v>
+      </c>
+      <c r="H9">
+        <v>-0.1681115327940939</v>
+      </c>
+      <c r="I9">
+        <v>0.1931208983274703</v>
+      </c>
+      <c r="J9">
+        <v>3.219081740896161</v>
       </c>
     </row>
   </sheetData>
@@ -606,7 +1002,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -667,7 +1063,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>NS</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -681,63 +1077,291 @@
         </is>
       </c>
       <c r="D2">
-        <v>-0.9590715907057723</v>
+        <v>-0.9550465537608072</v>
       </c>
       <c r="E2">
-        <v>0.8169016176624994</v>
+        <v>0.7121295874003903</v>
       </c>
       <c r="F2">
-        <v>-2.367727920020121</v>
+        <v>-2.648774833463925</v>
       </c>
       <c r="G2">
-        <v>0.03170726890415806</v>
+        <v>0.01709637891534892</v>
       </c>
       <c r="H2">
-        <v>-0.9987151674845285</v>
+        <v>-0.997735311323387</v>
       </c>
       <c r="I2">
-        <v>-0.1912032725156168</v>
+        <v>-0.3639016506019306</v>
       </c>
       <c r="J2">
-        <v>15.05657089176661</v>
+        <v>16.64665398949977</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>AT</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>std_error</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>summary</t>
+        </is>
+      </c>
+      <c r="D3">
+        <v>-0.8832873330083435</v>
+      </c>
+      <c r="E3">
+        <v>0.7926051751144784</v>
+      </c>
+      <c r="F3">
+        <v>-1.754378548699929</v>
+      </c>
+      <c r="G3">
+        <v>0.1163723842246377</v>
+      </c>
+      <c r="H3">
+        <v>-0.9967429741369245</v>
+      </c>
+      <c r="I3">
+        <v>0.4037908529076468</v>
+      </c>
+      <c r="J3">
+        <v>8.23532585079065</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CS</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>std_error</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>summary</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>-0.7611348872908961</v>
+      </c>
+      <c r="E4">
+        <v>0.807246403611002</v>
+      </c>
+      <c r="F4">
+        <v>-1.237425575991116</v>
+      </c>
+      <c r="G4">
+        <v>0.2746410859944678</v>
+      </c>
+      <c r="H4">
+        <v>-0.9961121816322973</v>
+      </c>
+      <c r="I4">
+        <v>0.808519715971413</v>
+      </c>
+      <c r="J4">
+        <v>4.658804338291473</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>CT</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>std_error</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>summary</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>0.3096685115952075</v>
+      </c>
+      <c r="E5">
+        <v>1.585054362032648</v>
+      </c>
+      <c r="F5">
+        <v>0.2019985732740182</v>
+      </c>
+      <c r="G5">
+        <v>0.8488035746742343</v>
+      </c>
+      <c r="H5">
+        <v>-0.9991929252578232</v>
+      </c>
+      <c r="I5">
+        <v>0.9997756981108061</v>
+      </c>
+      <c r="J5">
+        <v>4.459581677819079</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>NS</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>std_error</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>summary</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>-0.8636774935235872</v>
+      </c>
+      <c r="E6">
+        <v>0.5617352514820125</v>
+      </c>
+      <c r="F6">
+        <v>-2.327861305888846</v>
+      </c>
+      <c r="G6">
+        <v>0.1519462634670303</v>
+      </c>
+      <c r="H6">
+        <v>-0.9990958173846504</v>
+      </c>
+      <c r="I6">
+        <v>0.8441108261553172</v>
+      </c>
+      <c r="J6">
+        <v>1.900070298458818</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>NT</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>std_error</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>summary</t>
         </is>
       </c>
-      <c r="D3">
-        <v>-0.810807298457497</v>
-      </c>
-      <c r="E3">
-        <v>0.5651875525398972</v>
-      </c>
-      <c r="F3">
-        <v>-1.998241075375389</v>
-      </c>
-      <c r="G3">
-        <v>0.07647123240499687</v>
-      </c>
-      <c r="H3">
-        <v>-0.9838708325249662</v>
-      </c>
-      <c r="I3">
-        <v>0.1462692590113416</v>
-      </c>
-      <c r="J3">
-        <v>9.085706055197749</v>
+      <c r="D7">
+        <v>-1</v>
+      </c>
+      <c r="E7">
+        <v>14.6593530178123</v>
+      </c>
+      <c r="F7">
+        <v>-3.594127301119653</v>
+      </c>
+      <c r="G7">
+        <v>0.05449854716300429</v>
+      </c>
+      <c r="H7">
+        <v>-1</v>
+      </c>
+      <c r="I7">
+        <v>0.977252113196392</v>
+      </c>
+      <c r="J7">
+        <v>2.347485225724891</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>RS</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>std_error</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>summary</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>-0.9143872882845433</v>
+      </c>
+      <c r="E8">
+        <v>2.910168408875418</v>
+      </c>
+      <c r="F8">
+        <v>-0.5338727328583842</v>
+      </c>
+      <c r="G8">
+        <v>0.6564523272410571</v>
+      </c>
+      <c r="H8">
+        <v>-0.9999999999999964</v>
+      </c>
+      <c r="I8">
+        <v>0.9999999999982374</v>
+      </c>
+      <c r="J8">
+        <v>1.651111386082563</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>RT</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>std_error</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>summary</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>-0.1304457439229121</v>
+      </c>
+      <c r="E9">
+        <v>0.9811360206807996</v>
+      </c>
+      <c r="F9">
+        <v>-0.1337156933533045</v>
+      </c>
+      <c r="G9">
+        <v>0.911428223938668</v>
+      </c>
+      <c r="H9">
+        <v>-0.9999994976922165</v>
+      </c>
+      <c r="I9">
+        <v>0.9999991510621278</v>
+      </c>
+      <c r="J9">
+        <v>1.288858588319265</v>
       </c>
     </row>
   </sheetData>
@@ -747,7 +1371,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -773,27 +1397,105 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>NS</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="B2">
-        <v>845</v>
+        <v>481</v>
       </c>
       <c r="C2">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>AT</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>278</v>
+      </c>
+      <c r="C3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CS</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>124</v>
+      </c>
+      <c r="C4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>CT</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>64</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>NS</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>67</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>RT</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>26</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>NT</t>
         </is>
       </c>
-      <c r="B3">
-        <v>438</v>
-      </c>
-      <c r="C3">
-        <v>51</v>
+      <c r="B8">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>RS</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>69</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>